<commit_message>
all changes corresponding to release v1.0.1
</commit_message>
<xml_diff>
--- a/processing/README.xlsx
+++ b/processing/README.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf8120b967e1a705/Documents/Work/CBF/Emmott_Annotation/Application/scpannotation/processingpy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf8120b967e1a705/Documents/Work/CBF/Emmott_Annotation/Application/scpannotation/processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBFF4F55-E280-4B17-BF34-1FE283E0F40F}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F03A32B3-B3B4-45B7-A2CB-D97BFE08D6A5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
   <si>
     <t>1G1,</t>
   </si>
@@ -185,12 +185,6 @@
     <t>Import either folder containing ".raw" files or CSV formatted like 'Raw File Import - Template'</t>
   </si>
   <si>
-    <t>Import .csv</t>
-  </si>
-  <si>
-    <t>Import as many .csv cell files as desired</t>
-  </si>
-  <si>
     <t>Handle Cell File Column Mismatches</t>
   </si>
   <si>
@@ -209,27 +203,15 @@
     <t>Choose how cell files should be named</t>
   </si>
   <si>
-    <t>Name TMT labels with no cell data</t>
-  </si>
-  <si>
     <t>Add extra rows per raw file</t>
   </si>
   <si>
     <t>Any extra rows to add per raw file</t>
   </si>
   <si>
-    <t>Well to TMT mapping CSV</t>
-  </si>
-  <si>
-    <t>Choose the mapping of well to TMT file, if default selected 'Well to TMT mapping - Default' is used, else 'Well to TMT mapping - Template' can be populated and uploaded as a csv</t>
-  </si>
-  <si>
     <t>Pickup type</t>
   </si>
   <si>
-    <t>Included for future compatibility, currently only single pickup is supported</t>
-  </si>
-  <si>
     <t>Page</t>
   </si>
   <si>
@@ -245,9 +227,6 @@
     <t>Tick columns to include in output file</t>
   </si>
   <si>
-    <t>Choose values for TMT labels with no cell data</t>
-  </si>
-  <si>
     <t>SCP Sample Annotation Wizard</t>
   </si>
   <si>
@@ -264,6 +243,39 @@
   </si>
   <si>
     <t>Editing the name of the application will lead to errors</t>
+  </si>
+  <si>
+    <t>Select whether data was generated from single pickup or dual pickup. If dual, then include the offset of the X position from the first position to the second</t>
+  </si>
+  <si>
+    <t>Import .log file or .log converted to csv</t>
+  </si>
+  <si>
+    <t>Import as many cell files as desired in .xls format, or converted to .csv</t>
+  </si>
+  <si>
+    <t>Assign a value to TMT labels or ({label free input file name}) that is currently missing cell data</t>
+  </si>
+  <si>
+    <t>Name missing cell data values</t>
+  </si>
+  <si>
+    <t>Technology used</t>
+  </si>
+  <si>
+    <t>Select the technology used to generate the data</t>
+  </si>
+  <si>
+    <t>Regex to extract row/ column</t>
+  </si>
+  <si>
+    <t>Edit the regex that is used to extract row and column names from raw file names if the default has failed to do so</t>
+  </si>
+  <si>
+    <t>Well to TMT mapping CSV (Only if TMT selected as technology)</t>
+  </si>
+  <si>
+    <t>Choose the mapping of well to TMT, if 'Default' selected 'Well to TMT mapping - Default' is used, else 'Well to TMT mapping - Template' can be populated and uploaded as a csv</t>
   </si>
 </sst>
 </file>
@@ -335,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -347,6 +359,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -363,6 +376,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -628,163 +645,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="162.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="162.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -796,13 +830,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
@@ -823,9 +857,9 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -833,7 +867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -841,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -849,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -857,7 +891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -865,7 +899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -873,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -881,7 +915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -889,7 +923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -897,7 +931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -905,7 +939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -913,7 +947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -921,7 +955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -929,7 +963,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -937,7 +971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -945,7 +979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -953,7 +987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -961,7 +995,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -969,7 +1003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -977,7 +1011,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -993,9 +1027,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1003,79 +1037,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
     </row>

</xml_diff>

<commit_message>
redesigned welltomapping csv to be more user friendly
</commit_message>
<xml_diff>
--- a/processing/README.xlsx
+++ b/processing/README.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf8120b967e1a705/Documents/Work/CBF/Emmott_Annotation/Application/scpannotation/processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F03A32B3-B3B4-45B7-A2CB-D97BFE08D6A5}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A085C16E-AFF7-413B-8E63-9B608BAE8922}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>1G1,</t>
   </si>
@@ -143,16 +143,10 @@
     <t>Reporter.intensity.2</t>
   </si>
   <si>
-    <t>Empty</t>
-  </si>
-  <si>
     <t>Reporter.intensity.3</t>
   </si>
   <si>
     <t>Reporter.intensity.4</t>
-  </si>
-  <si>
-    <t>Control</t>
   </si>
   <si>
     <t>RawFileName</t>
@@ -347,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -359,7 +353,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -647,173 +640,173 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="162.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="162.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="M11" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>65</v>
-      </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -830,18 +823,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -853,13 +846,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94668D3-9B44-4A18-A015-FDD060A91080}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -867,7 +860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -875,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -883,7 +876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -891,7 +884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -899,7 +892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -907,7 +900,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -915,7 +908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -923,7 +916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -931,7 +924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -939,7 +932,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -947,7 +940,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -955,7 +948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -963,7 +956,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -971,7 +964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -979,7 +972,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -987,7 +980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -995,26 +988,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1027,9 +1014,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1037,79 +1024,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
     </row>

</xml_diff>

<commit_message>
improved user friendliness of welltomapping.csv, reporters not present - filled missing value label,  added tmt labelling offset
</commit_message>
<xml_diff>
--- a/processing/README.xlsx
+++ b/processing/README.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf8120b967e1a705/Documents/Work/CBF/Emmott_Annotation/Application/scpannotation/processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A085C16E-AFF7-413B-8E63-9B608BAE8922}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1888E6C-FD3F-409A-97DB-2784ED3D9357}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>Add extra rows per raw file</t>
   </si>
   <si>
-    <t>Any extra rows to add per raw file</t>
-  </si>
-  <si>
     <t>Pickup type</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>Choose the mapping of well to TMT, if 'Default' selected 'Well to TMT mapping - Default' is used, else 'Well to TMT mapping - Template' can be populated and uploaded as a csv</t>
+  </si>
+  <si>
+    <t>Add extra rows per raw file, in addition to the labels given to missing data defined above</t>
   </si>
 </sst>
 </file>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,28 +653,28 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -682,10 +682,10 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
         <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -709,7 +709,7 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -717,15 +717,15 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
         <v>62</v>
-      </c>
-      <c r="C11" t="s">
-        <v>63</v>
       </c>
       <c r="M11" s="4"/>
     </row>
@@ -734,10 +734,10 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
         <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -745,7 +745,7 @@
         <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -769,10 +769,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -780,33 +780,33 @@
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94668D3-9B44-4A18-A015-FDD060A91080}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pickup and raw files now match on well, not col and row
</commit_message>
<xml_diff>
--- a/processing/README.xlsx
+++ b/processing/README.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf8120b967e1a705/Documents/Work/CBF/Emmott_Annotation/Application/scpannotation/processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1888E6C-FD3F-409A-97DB-2784ED3D9357}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AF8BC3F-2A4A-4246-A916-CA3AA0508A20}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="Raw File Import - Template" sheetId="4" r:id="rId2"/>
-    <sheet name="Well to TMT mapping - Default" sheetId="2" r:id="rId3"/>
-    <sheet name="Well to TMT mapping - Template" sheetId="3" r:id="rId4"/>
+    <sheet name="Well to Label mapping - Default" sheetId="2" r:id="rId3"/>
+    <sheet name="Well to Label mapping -Template" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>1G1,</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Well</t>
   </si>
   <si>
-    <t>TMT</t>
-  </si>
-  <si>
     <t>1G10,</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Raw files</t>
   </si>
   <si>
-    <t>Labels file</t>
-  </si>
-  <si>
     <t>Import Page</t>
   </si>
   <si>
@@ -245,9 +239,6 @@
     <t>Import as many cell files as desired in .xls format, or converted to .csv</t>
   </si>
   <si>
-    <t>Assign a value to TMT labels or ({label free input file name}) that is currently missing cell data</t>
-  </si>
-  <si>
     <t>Name missing cell data values</t>
   </si>
   <si>
@@ -263,13 +254,25 @@
     <t>Edit the regex that is used to extract row and column names from raw file names if the default has failed to do so</t>
   </si>
   <si>
-    <t>Well to TMT mapping CSV (Only if TMT selected as technology)</t>
-  </si>
-  <si>
-    <t>Choose the mapping of well to TMT, if 'Default' selected 'Well to TMT mapping - Default' is used, else 'Well to TMT mapping - Template' can be populated and uploaded as a csv</t>
-  </si>
-  <si>
     <t>Add extra rows per raw file, in addition to the labels given to missing data defined above</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Well to Label mapping CSV (Only if "Label-based" selected as technology)</t>
+  </si>
+  <si>
+    <t>Choose the mapping of well to Label, if 'Default' selected 'Well to Label mapping - Default' is used, else 'Well to Label mapping - Template' can be populated and uploaded as a csv</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Labels file / droplet location file</t>
+  </si>
+  <si>
+    <t>Assign a value to wells that are missing cell data</t>
   </si>
 </sst>
 </file>
@@ -641,172 +644,172 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="162.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M11" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
         <v>74</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -831,10 +834,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -847,157 +850,161 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1012,7 +1019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD111AF-F29C-4736-ABB1-D5283293FAD9}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1021,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update documentation and tooltips
</commit_message>
<xml_diff>
--- a/processing/README.xlsx
+++ b/processing/README.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf8120b967e1a705/Documents/Work/CBF/Emmott_Annotation/Application/scpannotation/processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AF8BC3F-2A4A-4246-A916-CA3AA0508A20}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{3259F599-D68F-46CF-B409-2DFBF7B21CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A1DCBF0-AFCB-45E7-8DBC-DDB06A8823EE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>1G1,</t>
   </si>
@@ -152,9 +152,6 @@
     <t>MSAquisDateTime</t>
   </si>
   <si>
-    <t>Raw files</t>
-  </si>
-  <si>
     <t>Import Page</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t>Edit the regex that is used to extract row and column names from raw file names if the default has failed to do so</t>
   </si>
   <si>
-    <t>Add extra rows per raw file, in addition to the labels given to missing data defined above</t>
-  </si>
-  <si>
     <t>Empty</t>
   </si>
   <si>
@@ -272,7 +266,43 @@
     <t>Labels file / droplet location file</t>
   </si>
   <si>
-    <t>Assign a value to wells that are missing cell data</t>
+    <t>Additional cellenONE annotation files</t>
+  </si>
+  <si>
+    <t>Import additional cellenONE annotation files in .fld format to include as an output column</t>
+  </si>
+  <si>
+    <t>Data files</t>
+  </si>
+  <si>
+    <t>Date File Extension</t>
+  </si>
+  <si>
+    <t>Select the type of data used</t>
+  </si>
+  <si>
+    <t>Regex to extract well</t>
+  </si>
+  <si>
+    <t>Enter regex to correctly extract well to merge cell files and data files</t>
+  </si>
+  <si>
+    <t>Enter a value to fill any missing row</t>
+  </si>
+  <si>
+    <t>Any extra rows to add per raw file</t>
+  </si>
+  <si>
+    <t>Well to TMT mapping CSV</t>
+  </si>
+  <si>
+    <t>Choose the mapping of well to TMT file, if default selected 'Well to TMT mapping - Default' is used, else 'Well to TMT mapping - Template' can be populated and uploaded as a csv</t>
+  </si>
+  <si>
+    <t>Invert numbering</t>
+  </si>
+  <si>
+    <t>Select whether the numbering of column or row should be inverted e.g. "3, 2, 1" instead of "1, 2, 3". And if so, enter the regex to correctly select the column or row.</t>
   </si>
 </sst>
 </file>
@@ -344,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -356,6 +386,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,52 +689,52 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
         <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
         <v>42</v>
@@ -709,107 +742,147 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="M13" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
         <v>69</v>
       </c>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -993,7 +1066,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
@@ -1001,7 +1074,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -1030,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>